<commit_message>
update excels with no index, update trust percentage log2excel
</commit_message>
<xml_diff>
--- a/excel/grouptc_bs_ablation_time.xlsx
+++ b/excel/grouptc_bs_ablation_time.xlsx
@@ -503,1190 +503,1082 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2">
+        <v>0.303</v>
+      </c>
       <c r="C2">
-        <v>0.303</v>
+        <v>0.297</v>
       </c>
       <c r="D2">
+        <v>0.277</v>
+      </c>
+      <c r="E2">
+        <v>0.278</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3.367003367003367</v>
+      </c>
+      <c r="H2">
+        <v>3.610108303249097</v>
+      </c>
+      <c r="I2">
+        <v>3.597122302158274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.208</v>
+      </c>
+      <c r="C3">
+        <v>0.188</v>
+      </c>
+      <c r="D3">
+        <v>0.17</v>
+      </c>
+      <c r="E3">
+        <v>0.179</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>5.319148936170213</v>
+      </c>
+      <c r="H3">
+        <v>5.88235294117647</v>
+      </c>
+      <c r="I3">
+        <v>5.58659217877095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>0.298</v>
+      </c>
+      <c r="C4">
         <v>0.297</v>
       </c>
-      <c r="E2">
-        <v>0.277</v>
-      </c>
-      <c r="F2">
+      <c r="D4">
         <v>0.278</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="E4">
+        <v>0.29</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>3.367003367003367</v>
       </c>
-      <c r="I2">
-        <v>3.610108303249097</v>
-      </c>
-      <c r="J2">
+      <c r="H4">
         <v>3.597122302158274</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>0.208</v>
-      </c>
-      <c r="D3">
-        <v>0.188</v>
-      </c>
-      <c r="E3">
-        <v>0.17</v>
-      </c>
-      <c r="F3">
-        <v>0.179</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>5.319148936170213</v>
-      </c>
-      <c r="I3">
-        <v>5.88235294117647</v>
-      </c>
-      <c r="J3">
-        <v>5.58659217877095</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>0.298</v>
-      </c>
-      <c r="D4">
-        <v>0.297</v>
-      </c>
-      <c r="E4">
-        <v>0.278</v>
-      </c>
-      <c r="F4">
-        <v>0.29</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>3.367003367003367</v>
-      </c>
       <c r="I4">
-        <v>3.597122302158274</v>
-      </c>
-      <c r="J4">
         <v>3.448275862068966</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
+      <c r="B5">
+        <v>0.248</v>
+      </c>
       <c r="C5">
-        <v>0.248</v>
+        <v>0.262</v>
       </c>
       <c r="D5">
-        <v>0.262</v>
+        <v>0.22</v>
       </c>
       <c r="E5">
-        <v>0.22</v>
+        <v>0.231</v>
       </c>
       <c r="F5">
-        <v>0.231</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>3.816793893129771</v>
       </c>
       <c r="H5">
-        <v>3.816793893129771</v>
+        <v>4.545454545454546</v>
       </c>
       <c r="I5">
-        <v>4.545454545454546</v>
-      </c>
-      <c r="J5">
         <v>4.329004329004329</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6">
+        <v>2.704</v>
+      </c>
       <c r="C6">
-        <v>2.704</v>
+        <v>2.276</v>
       </c>
       <c r="D6">
-        <v>2.276</v>
+        <v>0.9079999999999999</v>
       </c>
       <c r="E6">
-        <v>0.9079999999999999</v>
+        <v>0.924</v>
       </c>
       <c r="F6">
-        <v>0.924</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.4393673110720563</v>
       </c>
       <c r="H6">
-        <v>0.4393673110720563</v>
+        <v>1.101321585903084</v>
       </c>
       <c r="I6">
-        <v>1.101321585903084</v>
-      </c>
-      <c r="J6">
         <v>1.082251082251082</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
+      <c r="B7">
+        <v>1.763</v>
+      </c>
       <c r="C7">
-        <v>1.763</v>
+        <v>1.74</v>
       </c>
       <c r="D7">
-        <v>1.74</v>
+        <v>1.378</v>
       </c>
       <c r="E7">
-        <v>1.378</v>
+        <v>1.389</v>
       </c>
       <c r="F7">
-        <v>1.389</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.5747126436781609</v>
       </c>
       <c r="H7">
-        <v>0.5747126436781609</v>
+        <v>0.7256894049346879</v>
       </c>
       <c r="I7">
-        <v>0.7256894049346879</v>
-      </c>
-      <c r="J7">
         <v>0.7199424046076314</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="B8">
+        <v>1.652</v>
+      </c>
       <c r="C8">
-        <v>1.652</v>
+        <v>1.57</v>
       </c>
       <c r="D8">
-        <v>1.57</v>
+        <v>1.513</v>
       </c>
       <c r="E8">
-        <v>1.513</v>
+        <v>1.608</v>
       </c>
       <c r="F8">
-        <v>1.608</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0.6369426751592356</v>
       </c>
       <c r="H8">
-        <v>0.6369426751592356</v>
+        <v>0.6609385327164573</v>
       </c>
       <c r="I8">
-        <v>0.6609385327164573</v>
-      </c>
-      <c r="J8">
         <v>0.6218905472636815</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
+      <c r="B9">
+        <v>3.133</v>
+      </c>
       <c r="C9">
-        <v>3.133</v>
+        <v>3.18</v>
       </c>
       <c r="D9">
-        <v>3.18</v>
+        <v>2.29</v>
       </c>
       <c r="E9">
-        <v>2.29</v>
+        <v>2.286</v>
       </c>
       <c r="F9">
-        <v>2.286</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0.3144654088050314</v>
       </c>
       <c r="H9">
-        <v>0.3144654088050314</v>
+        <v>0.4366812227074236</v>
       </c>
       <c r="I9">
-        <v>0.4366812227074236</v>
-      </c>
-      <c r="J9">
         <v>0.4374453193350831</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="B10">
+        <v>5.244999999999999</v>
+      </c>
       <c r="C10">
-        <v>5.244999999999999</v>
+        <v>4.33</v>
       </c>
       <c r="D10">
-        <v>4.33</v>
+        <v>4.114999999999999</v>
       </c>
       <c r="E10">
-        <v>4.114999999999999</v>
+        <v>4.189</v>
       </c>
       <c r="F10">
-        <v>4.189</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0.2309468822170901</v>
       </c>
       <c r="H10">
-        <v>0.2309468822170901</v>
+        <v>0.2430133657351155</v>
       </c>
       <c r="I10">
-        <v>0.2430133657351155</v>
-      </c>
-      <c r="J10">
         <v>0.23872045834328</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
+      <c r="B11">
+        <v>8.254</v>
+      </c>
       <c r="C11">
-        <v>8.254</v>
+        <v>7.674</v>
       </c>
       <c r="D11">
-        <v>7.674</v>
+        <v>8.243</v>
       </c>
       <c r="E11">
-        <v>8.243</v>
+        <v>8.363000000000001</v>
       </c>
       <c r="F11">
-        <v>8.363000000000001</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0.1303101381287464</v>
       </c>
       <c r="H11">
-        <v>0.1303101381287464</v>
+        <v>0.1213150551983501</v>
       </c>
       <c r="I11">
-        <v>0.1213150551983501</v>
-      </c>
-      <c r="J11">
         <v>0.1195743154370441</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
+      <c r="B12">
+        <v>32.822</v>
+      </c>
       <c r="C12">
-        <v>32.822</v>
+        <v>29.091</v>
       </c>
       <c r="D12">
-        <v>29.091</v>
+        <v>20.512</v>
       </c>
       <c r="E12">
-        <v>20.512</v>
+        <v>20.367</v>
       </c>
       <c r="F12">
-        <v>20.367</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0.03437489257846069</v>
       </c>
       <c r="H12">
-        <v>0.03437489257846069</v>
+        <v>0.04875195007800312</v>
       </c>
       <c r="I12">
-        <v>0.04875195007800312</v>
-      </c>
-      <c r="J12">
         <v>0.04909903274905484</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
+      <c r="B13">
+        <v>12.667</v>
+      </c>
       <c r="C13">
-        <v>12.667</v>
+        <v>13.384</v>
       </c>
       <c r="D13">
-        <v>13.384</v>
+        <v>13.425</v>
       </c>
       <c r="E13">
-        <v>13.425</v>
+        <v>13.381</v>
       </c>
       <c r="F13">
-        <v>13.381</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0.07471607890017931</v>
       </c>
       <c r="H13">
-        <v>0.07471607890017931</v>
+        <v>0.074487895716946</v>
       </c>
       <c r="I13">
-        <v>0.074487895716946</v>
-      </c>
-      <c r="J13">
         <v>0.07473283013227711</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
+      <c r="B14">
+        <v>18.41</v>
+      </c>
       <c r="C14">
-        <v>18.41</v>
+        <v>18.893</v>
       </c>
       <c r="D14">
-        <v>18.893</v>
+        <v>18.497</v>
       </c>
       <c r="E14">
-        <v>18.497</v>
+        <v>18.414</v>
       </c>
       <c r="F14">
-        <v>18.414</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0.0529296564865294</v>
       </c>
       <c r="H14">
-        <v>0.0529296564865294</v>
+        <v>0.05406282099799967</v>
       </c>
       <c r="I14">
-        <v>0.05406282099799967</v>
-      </c>
-      <c r="J14">
         <v>0.05430650591940914</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
+      <c r="B15">
+        <v>5.384</v>
+      </c>
       <c r="C15">
-        <v>5.384</v>
+        <v>5.565</v>
       </c>
       <c r="D15">
-        <v>5.565</v>
+        <v>5.035</v>
       </c>
       <c r="E15">
-        <v>5.035</v>
+        <v>5.046</v>
       </c>
       <c r="F15">
-        <v>5.046</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0.1796945193171609</v>
       </c>
       <c r="H15">
-        <v>0.1796945193171609</v>
+        <v>0.198609731876862</v>
       </c>
       <c r="I15">
-        <v>0.198609731876862</v>
-      </c>
-      <c r="J15">
         <v>0.1981767736821244</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
+      <c r="B16">
+        <v>427.977</v>
+      </c>
       <c r="C16">
-        <v>427.977</v>
+        <v>382.132</v>
       </c>
       <c r="D16">
-        <v>382.132</v>
+        <v>257.77</v>
       </c>
       <c r="E16">
-        <v>257.77</v>
+        <v>252.78</v>
       </c>
       <c r="F16">
-        <v>252.78</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0.002616896779123444</v>
       </c>
       <c r="H16">
-        <v>0.002616896779123444</v>
+        <v>0.003879427396516275</v>
       </c>
       <c r="I16">
-        <v>0.003879427396516275</v>
-      </c>
-      <c r="J16">
         <v>0.003956009177941293</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
+      <c r="B17">
+        <v>111.56</v>
+      </c>
       <c r="C17">
-        <v>111.56</v>
+        <v>101.745</v>
       </c>
       <c r="D17">
-        <v>101.745</v>
+        <v>95.12700000000001</v>
       </c>
       <c r="E17">
-        <v>95.12700000000001</v>
+        <v>94.874</v>
       </c>
       <c r="F17">
-        <v>94.874</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0.009828492800629023</v>
       </c>
       <c r="H17">
-        <v>0.009828492800629023</v>
+        <v>0.01051226255426956</v>
       </c>
       <c r="I17">
-        <v>0.01051226255426956</v>
-      </c>
-      <c r="J17">
         <v>0.01054029554988722</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
+      <c r="B18">
+        <v>116.981</v>
+      </c>
       <c r="C18">
-        <v>116.981</v>
+        <v>109.073</v>
       </c>
       <c r="D18">
-        <v>109.073</v>
+        <v>98.895</v>
       </c>
       <c r="E18">
-        <v>98.895</v>
+        <v>98.66500000000001</v>
       </c>
       <c r="F18">
-        <v>98.66500000000001</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0.009168171774866373</v>
       </c>
       <c r="H18">
-        <v>0.009168171774866373</v>
+        <v>0.01011173466808231</v>
       </c>
       <c r="I18">
-        <v>0.01011173466808231</v>
-      </c>
-      <c r="J18">
         <v>0.01013530633963411</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
+      <c r="B19">
+        <v>16.861</v>
+      </c>
       <c r="C19">
-        <v>16.861</v>
+        <v>16.723</v>
       </c>
       <c r="D19">
-        <v>16.723</v>
+        <v>15.552</v>
       </c>
       <c r="E19">
-        <v>15.552</v>
+        <v>15.744</v>
       </c>
       <c r="F19">
-        <v>15.744</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.05979788315493632</v>
       </c>
       <c r="H19">
-        <v>0.05979788315493632</v>
+        <v>0.06430041152263374</v>
       </c>
       <c r="I19">
-        <v>0.06430041152263374</v>
-      </c>
-      <c r="J19">
         <v>0.06351626016260162</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
+      <c r="B20">
+        <v>5068.971</v>
+      </c>
       <c r="C20">
-        <v>5068.971</v>
+        <v>4499.527</v>
       </c>
       <c r="D20">
-        <v>4499.527</v>
+        <v>3170.485</v>
       </c>
       <c r="E20">
-        <v>3170.485</v>
+        <v>3055.351</v>
       </c>
       <c r="F20">
-        <v>3055.351</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0.0002222455827023596</v>
       </c>
       <c r="H20">
-        <v>0.0002222455827023596</v>
+        <v>0.0003154091566432265</v>
       </c>
       <c r="I20">
-        <v>0.0003154091566432265</v>
-      </c>
-      <c r="J20">
         <v>0.0003272946381610492</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
         <v>28</v>
       </c>
+      <c r="B21">
+        <v>2541.915</v>
+      </c>
       <c r="C21">
-        <v>2541.915</v>
+        <v>2258.984</v>
       </c>
       <c r="D21">
-        <v>2258.984</v>
+        <v>2188.833</v>
       </c>
       <c r="E21">
-        <v>2188.833</v>
+        <v>2176.627</v>
       </c>
       <c r="F21">
-        <v>2176.627</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0.0004426768848296403</v>
       </c>
       <c r="H21">
-        <v>0.0004426768848296403</v>
+        <v>0.000456864456996034</v>
       </c>
       <c r="I21">
-        <v>0.000456864456996034</v>
-      </c>
-      <c r="J21">
         <v>0.0004594264428402294</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
+      <c r="B22">
+        <v>1.382</v>
+      </c>
       <c r="C22">
-        <v>1.382</v>
+        <v>1.119</v>
       </c>
       <c r="D22">
-        <v>1.119</v>
+        <v>0.574</v>
       </c>
       <c r="E22">
-        <v>0.574</v>
+        <v>0.5760000000000001</v>
       </c>
       <c r="F22">
-        <v>0.5760000000000001</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0.8936550491510277</v>
       </c>
       <c r="H22">
-        <v>0.8936550491510277</v>
+        <v>1.742160278745645</v>
       </c>
       <c r="I22">
-        <v>1.742160278745645</v>
-      </c>
-      <c r="J22">
         <v>1.736111111111111</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
+      <c r="B23">
+        <v>5.502</v>
+      </c>
       <c r="C23">
-        <v>5.502</v>
+        <v>4.460999999999999</v>
       </c>
       <c r="D23">
-        <v>4.460999999999999</v>
+        <v>2.236</v>
       </c>
       <c r="E23">
-        <v>2.236</v>
+        <v>2.24</v>
       </c>
       <c r="F23">
-        <v>2.24</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0.224164985429276</v>
       </c>
       <c r="H23">
-        <v>0.224164985429276</v>
+        <v>0.4472271914132379</v>
       </c>
       <c r="I23">
-        <v>0.4472271914132379</v>
-      </c>
-      <c r="J23">
         <v>0.4464285714285715</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
+      <c r="B24">
+        <v>17.121</v>
+      </c>
       <c r="C24">
-        <v>17.121</v>
+        <v>15.129</v>
       </c>
       <c r="D24">
-        <v>15.129</v>
+        <v>8.063000000000001</v>
       </c>
       <c r="E24">
-        <v>8.063000000000001</v>
+        <v>8.061</v>
       </c>
       <c r="F24">
-        <v>8.061</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0.06609822195782934</v>
       </c>
       <c r="H24">
-        <v>0.06609822195782934</v>
+        <v>0.1240233163834801</v>
       </c>
       <c r="I24">
-        <v>0.1240233163834801</v>
-      </c>
-      <c r="J24">
         <v>0.1240540875821858</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
+      <c r="B25">
+        <v>53.499</v>
+      </c>
       <c r="C25">
-        <v>53.499</v>
+        <v>47.155</v>
       </c>
       <c r="D25">
-        <v>47.155</v>
+        <v>27.701</v>
       </c>
       <c r="E25">
-        <v>27.701</v>
+        <v>27.2</v>
       </c>
       <c r="F25">
-        <v>27.2</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0.02120665889089174</v>
       </c>
       <c r="H25">
-        <v>0.02120665889089174</v>
+        <v>0.03609977979134327</v>
       </c>
       <c r="I25">
-        <v>0.03609977979134327</v>
-      </c>
-      <c r="J25">
         <v>0.03676470588235294</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
+      <c r="B26">
+        <v>181.606</v>
+      </c>
       <c r="C26">
-        <v>181.606</v>
+        <v>161.842</v>
       </c>
       <c r="D26">
-        <v>161.842</v>
+        <v>95.831</v>
       </c>
       <c r="E26">
-        <v>95.831</v>
+        <v>94.155</v>
       </c>
       <c r="F26">
-        <v>94.155</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0.006178865807392395</v>
       </c>
       <c r="H26">
-        <v>0.006178865807392395</v>
+        <v>0.01043503667915393</v>
       </c>
       <c r="I26">
-        <v>0.01043503667915393</v>
-      </c>
-      <c r="J26">
         <v>0.01062078487600234</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
+      <c r="B27">
+        <v>584.978</v>
+      </c>
       <c r="C27">
-        <v>584.978</v>
+        <v>526.1700000000001</v>
       </c>
       <c r="D27">
-        <v>526.1700000000001</v>
+        <v>320.481</v>
       </c>
       <c r="E27">
-        <v>320.481</v>
+        <v>302.929</v>
       </c>
       <c r="F27">
-        <v>302.929</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0.001900526445825493</v>
       </c>
       <c r="H27">
-        <v>0.001900526445825493</v>
+        <v>0.003120309784355391</v>
       </c>
       <c r="I27">
-        <v>0.003120309784355391</v>
-      </c>
-      <c r="J27">
         <v>0.003301103558919747</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
         <v>35</v>
       </c>
+      <c r="B28">
+        <v>1828.414</v>
+      </c>
       <c r="C28">
-        <v>1828.414</v>
+        <v>1656.266</v>
       </c>
       <c r="D28">
-        <v>1656.266</v>
+        <v>1036.003</v>
       </c>
       <c r="E28">
-        <v>1036.003</v>
+        <v>966.813</v>
       </c>
       <c r="F28">
-        <v>966.813</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0.0006037677522813365</v>
       </c>
       <c r="H28">
-        <v>0.0006037677522813365</v>
+        <v>0.0009652481701307816</v>
       </c>
       <c r="I28">
-        <v>0.0009652481701307816</v>
-      </c>
-      <c r="J28">
         <v>0.00103432618303643</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
         <v>36</v>
       </c>
+      <c r="B29">
+        <v>5486.331</v>
+      </c>
       <c r="C29">
-        <v>5486.331</v>
+        <v>4970.398</v>
       </c>
       <c r="D29">
-        <v>4970.398</v>
+        <v>3143.581</v>
       </c>
       <c r="E29">
-        <v>3143.581</v>
+        <v>2993.987</v>
       </c>
       <c r="F29">
-        <v>2993.987</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0.0002011911319777611</v>
       </c>
       <c r="H29">
-        <v>0.0002011911319777611</v>
+        <v>0.0003181085519985011</v>
       </c>
       <c r="I29">
-        <v>0.0003181085519985011</v>
-      </c>
-      <c r="J29">
         <v>0.0003340027862512429</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
         <v>37</v>
       </c>
+      <c r="B30">
+        <v>12.32</v>
+      </c>
       <c r="C30">
-        <v>12.32</v>
+        <v>10.863</v>
       </c>
       <c r="D30">
-        <v>10.863</v>
+        <v>6.26</v>
       </c>
       <c r="E30">
-        <v>6.26</v>
+        <v>6.207</v>
       </c>
       <c r="F30">
-        <v>6.207</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0.09205560158335635</v>
       </c>
       <c r="H30">
-        <v>0.09205560158335635</v>
+        <v>0.1597444089456869</v>
       </c>
       <c r="I30">
-        <v>0.1597444089456869</v>
-      </c>
-      <c r="J30">
         <v>0.1611084259706783</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
+      <c r="B31">
+        <v>28.612</v>
+      </c>
       <c r="C31">
-        <v>28.612</v>
+        <v>26.2</v>
       </c>
       <c r="D31">
-        <v>26.2</v>
+        <v>14.914</v>
       </c>
       <c r="E31">
-        <v>14.914</v>
+        <v>14.811</v>
       </c>
       <c r="F31">
-        <v>14.811</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0.0381679389312977</v>
       </c>
       <c r="H31">
-        <v>0.0381679389312977</v>
+        <v>0.0670510929328148</v>
       </c>
       <c r="I31">
-        <v>0.0670510929328148</v>
-      </c>
-      <c r="J31">
         <v>0.06751738572682466</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
+      <c r="B32">
+        <v>72.336</v>
+      </c>
       <c r="C32">
-        <v>72.336</v>
+        <v>63.44900000000001</v>
       </c>
       <c r="D32">
-        <v>63.44900000000001</v>
+        <v>37.40799999999999</v>
       </c>
       <c r="E32">
-        <v>37.40799999999999</v>
+        <v>36.865</v>
       </c>
       <c r="F32">
-        <v>36.865</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0.01576068968778074</v>
       </c>
       <c r="H32">
-        <v>0.01576068968778074</v>
+        <v>0.02673224978614201</v>
       </c>
       <c r="I32">
-        <v>0.02673224978614201</v>
-      </c>
-      <c r="J32">
         <v>0.02712600027126</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
         <v>33</v>
       </c>
+      <c r="B33">
+        <v>183.388</v>
+      </c>
       <c r="C33">
-        <v>183.388</v>
+        <v>162.605</v>
       </c>
       <c r="D33">
-        <v>162.605</v>
+        <v>95.72200000000001</v>
       </c>
       <c r="E33">
-        <v>95.72200000000001</v>
+        <v>94.196</v>
       </c>
       <c r="F33">
-        <v>94.196</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0.006149872390147905</v>
       </c>
       <c r="H33">
-        <v>0.006149872390147905</v>
+        <v>0.01044691920352688</v>
       </c>
       <c r="I33">
-        <v>0.01044691920352688</v>
-      </c>
-      <c r="J33">
         <v>0.01061616204509746</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
+      <c r="B34">
+        <v>480.624</v>
+      </c>
       <c r="C34">
-        <v>480.624</v>
+        <v>420.96</v>
       </c>
       <c r="D34">
-        <v>420.96</v>
+        <v>253.678</v>
       </c>
       <c r="E34">
-        <v>253.678</v>
+        <v>243.673</v>
       </c>
       <c r="F34">
-        <v>243.673</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0.002375522614975295</v>
       </c>
       <c r="H34">
-        <v>0.002375522614975295</v>
+        <v>0.00394200521921491</v>
       </c>
       <c r="I34">
-        <v>0.00394200521921491</v>
-      </c>
-      <c r="J34">
         <v>0.00410386050157383</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
+      <c r="B35">
+        <v>1246.001</v>
+      </c>
       <c r="C35">
-        <v>1246.001</v>
+        <v>1101.784</v>
       </c>
       <c r="D35">
-        <v>1101.784</v>
+        <v>656.4349999999999</v>
       </c>
       <c r="E35">
-        <v>656.4349999999999</v>
+        <v>628.929</v>
       </c>
       <c r="F35">
-        <v>628.929</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0.0009076189162304044</v>
       </c>
       <c r="H35">
-        <v>0.0009076189162304044</v>
+        <v>0.00152338007571199</v>
       </c>
       <c r="I35">
-        <v>0.00152338007571199</v>
-      </c>
-      <c r="J35">
         <v>0.00159000459511328</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
         <v>42</v>
       </c>
+      <c r="B36">
+        <v>3276.041</v>
+      </c>
       <c r="C36">
-        <v>3276.041</v>
+        <v>2859.348</v>
       </c>
       <c r="D36">
-        <v>2859.348</v>
+        <v>1706.758</v>
       </c>
       <c r="E36">
-        <v>1706.758</v>
+        <v>1641.911</v>
       </c>
       <c r="F36">
-        <v>1641.911</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0.0003497300783255483</v>
       </c>
       <c r="H36">
-        <v>0.0003497300783255483</v>
+        <v>0.0005859061448664661</v>
       </c>
       <c r="I36">
-        <v>0.0005859061448664661</v>
-      </c>
-      <c r="J36">
         <v>0.0006090464099454843</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
         <v>43</v>
       </c>
+      <c r="B37">
+        <v>8494.576999999999</v>
+      </c>
       <c r="C37">
-        <v>8494.576999999999</v>
+        <v>7428.715</v>
       </c>
       <c r="D37">
-        <v>7428.715</v>
+        <v>4343.467000000001</v>
       </c>
       <c r="E37">
-        <v>4343.467000000001</v>
+        <v>4257.93</v>
       </c>
       <c r="F37">
-        <v>4257.93</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>0.0001346127829644831</v>
       </c>
       <c r="H37">
-        <v>0.0001346127829644831</v>
+        <v>0.0002302308271249672</v>
       </c>
       <c r="I37">
-        <v>0.0002302308271249672</v>
-      </c>
-      <c r="J37">
         <v>0.0002348559041600026</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update grouptc_bs_ablation and all datasets excel
</commit_message>
<xml_diff>
--- a/excel/grouptc_bs_ablation_time.xlsx
+++ b/excel/grouptc_bs_ablation_time.xlsx
@@ -558,13 +558,13 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>3.367003367003367</v>
+        <v>1.02020202020202</v>
       </c>
       <c r="H2">
-        <v>3.610108303249097</v>
+        <v>1.093862815884476</v>
       </c>
       <c r="I2">
-        <v>3.597122302158274</v>
+        <v>1.089928057553957</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -587,13 +587,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>5.319148936170213</v>
+        <v>1.106382978723404</v>
       </c>
       <c r="H3">
-        <v>5.88235294117647</v>
+        <v>1.223529411764706</v>
       </c>
       <c r="I3">
-        <v>5.58659217877095</v>
+        <v>1.162011173184358</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -616,13 +616,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>3.367003367003367</v>
+        <v>1.003367003367003</v>
       </c>
       <c r="H4">
-        <v>3.597122302158274</v>
+        <v>1.071942446043165</v>
       </c>
       <c r="I4">
-        <v>3.448275862068966</v>
+        <v>1.027586206896552</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -645,13 +645,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>3.816793893129771</v>
+        <v>0.9465648854961831</v>
       </c>
       <c r="H5">
-        <v>4.545454545454546</v>
+        <v>1.127272727272727</v>
       </c>
       <c r="I5">
-        <v>4.329004329004329</v>
+        <v>1.073593073593073</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -674,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.4393673110720563</v>
+        <v>1.18804920913884</v>
       </c>
       <c r="H6">
-        <v>1.101321585903084</v>
+        <v>2.977973568281938</v>
       </c>
       <c r="I6">
-        <v>1.082251082251082</v>
+        <v>2.926406926406926</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -703,13 +703,13 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.5747126436781609</v>
+        <v>1.013218390804598</v>
       </c>
       <c r="H7">
-        <v>0.7256894049346879</v>
+        <v>1.279390420899855</v>
       </c>
       <c r="I7">
-        <v>0.7199424046076314</v>
+        <v>1.269258459323254</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -732,13 +732,13 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0.6369426751592356</v>
+        <v>1.052229299363057</v>
       </c>
       <c r="H8">
-        <v>0.6609385327164573</v>
+        <v>1.091870456047588</v>
       </c>
       <c r="I8">
-        <v>0.6218905472636815</v>
+        <v>1.027363184079602</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -761,13 +761,13 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0.3144654088050314</v>
+        <v>0.9852201257861635</v>
       </c>
       <c r="H9">
-        <v>0.4366812227074236</v>
+        <v>1.368122270742358</v>
       </c>
       <c r="I9">
-        <v>0.4374453193350831</v>
+        <v>1.370516185476815</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -790,13 +790,13 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0.2309468822170901</v>
+        <v>1.211316397228637</v>
       </c>
       <c r="H10">
-        <v>0.2430133657351155</v>
+        <v>1.27460510328068</v>
       </c>
       <c r="I10">
-        <v>0.23872045834328</v>
+        <v>1.252088804010504</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -819,13 +819,13 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.1303101381287464</v>
+        <v>1.075579880114673</v>
       </c>
       <c r="H11">
-        <v>0.1213150551983501</v>
+        <v>1.001334465607182</v>
       </c>
       <c r="I11">
-        <v>0.1195743154370441</v>
+        <v>0.986966399617362</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -848,13 +848,13 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0.03437489257846069</v>
+        <v>1.128252724210237</v>
       </c>
       <c r="H12">
-        <v>0.04875195007800312</v>
+        <v>1.600136505460218</v>
       </c>
       <c r="I12">
-        <v>0.04909903274905484</v>
+        <v>1.611528452889478</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -877,13 +877,13 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0.07471607890017931</v>
+        <v>0.9464285714285714</v>
       </c>
       <c r="H13">
-        <v>0.074487895716946</v>
+        <v>0.943538175046555</v>
       </c>
       <c r="I13">
-        <v>0.07473283013227711</v>
+        <v>0.9466407592855541</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -906,13 +906,13 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0.0529296564865294</v>
+        <v>0.9744349759170062</v>
       </c>
       <c r="H14">
-        <v>0.05406282099799967</v>
+        <v>0.995296534573174</v>
       </c>
       <c r="I14">
-        <v>0.05430650591940914</v>
+        <v>0.9997827739763223</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -935,13 +935,13 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>0.1796945193171609</v>
+        <v>0.9674752920035941</v>
       </c>
       <c r="H15">
-        <v>0.198609731876862</v>
+        <v>1.069314796425025</v>
       </c>
       <c r="I15">
-        <v>0.1981767736821244</v>
+        <v>1.066983749504558</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -964,13 +964,13 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>0.002616896779123444</v>
+        <v>1.119971632838914</v>
       </c>
       <c r="H16">
-        <v>0.003879427396516275</v>
+        <v>1.660305698878846</v>
       </c>
       <c r="I16">
-        <v>0.003956009177941293</v>
+        <v>1.693080939947781</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -993,13 +993,13 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0.009828492800629023</v>
+        <v>1.096466656838174</v>
       </c>
       <c r="H17">
-        <v>0.01051226255426956</v>
+        <v>1.172748010554312</v>
       </c>
       <c r="I17">
-        <v>0.01054029554988722</v>
+        <v>1.175875371545418</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1022,13 +1022,13 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0.009168171774866373</v>
+        <v>1.072501902395643</v>
       </c>
       <c r="H18">
-        <v>0.01011173466808231</v>
+        <v>1.182880833206937</v>
       </c>
       <c r="I18">
-        <v>0.01013530633963411</v>
+        <v>1.185638270916738</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1051,13 +1051,13 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>0.05979788315493632</v>
+        <v>1.008252107875381</v>
       </c>
       <c r="H19">
-        <v>0.06430041152263374</v>
+        <v>1.084169238683128</v>
       </c>
       <c r="I19">
-        <v>0.06351626016260162</v>
+        <v>1.070947662601626</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1080,13 +1080,13 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.0002222455827023596</v>
+        <v>1.126556413596363</v>
       </c>
       <c r="H20">
-        <v>0.0003154091566432265</v>
+        <v>1.598799868158973</v>
       </c>
       <c r="I20">
-        <v>0.0003272946381610492</v>
+        <v>1.659047029293852</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1109,13 +1109,13 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>0.0004426768848296403</v>
+        <v>1.125247013701735</v>
       </c>
       <c r="H21">
-        <v>0.000456864456996034</v>
+        <v>1.161310616205074</v>
       </c>
       <c r="I21">
-        <v>0.0004594264428402294</v>
+        <v>1.167822966452222</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1138,13 +1138,13 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0.8936550491510277</v>
+        <v>1.23503127792672</v>
       </c>
       <c r="H22">
-        <v>1.742160278745645</v>
+        <v>2.407665505226481</v>
       </c>
       <c r="I22">
-        <v>1.736111111111111</v>
+        <v>2.399305555555555</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1167,13 +1167,13 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0.224164985429276</v>
+        <v>1.233355749831876</v>
       </c>
       <c r="H23">
-        <v>0.4472271914132379</v>
+        <v>2.460644007155635</v>
       </c>
       <c r="I23">
-        <v>0.4464285714285715</v>
+        <v>2.45625</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1196,13 +1196,13 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <v>0.06609822195782934</v>
+        <v>1.131667658139996</v>
       </c>
       <c r="H24">
-        <v>0.1240233163834801</v>
+        <v>2.123403199801563</v>
       </c>
       <c r="I24">
-        <v>0.1240540875821858</v>
+        <v>2.123930033494604</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1225,13 +1225,13 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>0.02120665889089174</v>
+        <v>1.134535044003817</v>
       </c>
       <c r="H25">
-        <v>0.03609977979134327</v>
+        <v>1.931302119057074</v>
       </c>
       <c r="I25">
-        <v>0.03676470588235294</v>
+        <v>1.966875</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1254,13 +1254,13 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0.006178865807392395</v>
+        <v>1.122119103817303</v>
       </c>
       <c r="H26">
-        <v>0.01043503667915393</v>
+        <v>1.895065271154428</v>
       </c>
       <c r="I26">
-        <v>0.01062078487600234</v>
+        <v>1.92879825819128</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>0.001900526445825493</v>
+        <v>1.111766159226105</v>
       </c>
       <c r="H27">
-        <v>0.003120309784355391</v>
+        <v>1.825312577032648</v>
       </c>
       <c r="I27">
-        <v>0.003301103558919747</v>
+        <v>1.931072957689755</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1312,13 +1312,13 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <v>0.0006037677522813365</v>
+        <v>1.103937411019728</v>
       </c>
       <c r="H28">
-        <v>0.0009652481701307816</v>
+        <v>1.764873267741503</v>
       </c>
       <c r="I28">
-        <v>0.00103432618303643</v>
+        <v>1.891176473630371</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1341,13 +1341,13 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <v>0.0002011911319777611</v>
+        <v>1.103801144294682</v>
       </c>
       <c r="H29">
-        <v>0.0003181085519985011</v>
+        <v>1.745248810194488</v>
       </c>
       <c r="I29">
-        <v>0.0003340027862512429</v>
+        <v>1.832449840296568</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1370,13 +1370,13 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>0.09205560158335635</v>
+        <v>1.13412501150695</v>
       </c>
       <c r="H30">
-        <v>0.1597444089456869</v>
+        <v>1.968051118210862</v>
       </c>
       <c r="I30">
-        <v>0.1611084259706783</v>
+        <v>1.984855807958756</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1399,13 +1399,13 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <v>0.0381679389312977</v>
+        <v>1.09206106870229</v>
       </c>
       <c r="H31">
-        <v>0.0670510929328148</v>
+        <v>1.918465870993697</v>
       </c>
       <c r="I31">
-        <v>0.06751738572682466</v>
+        <v>1.931807440415907</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1428,13 +1428,13 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <v>0.01576068968778074</v>
+        <v>1.140065249255307</v>
       </c>
       <c r="H32">
-        <v>0.02673224978614201</v>
+        <v>1.933704020530368</v>
       </c>
       <c r="I32">
-        <v>0.02712600027126</v>
+        <v>1.962186355621863</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1457,13 +1457,13 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <v>0.006149872390147905</v>
+        <v>1.127812797884444</v>
       </c>
       <c r="H33">
-        <v>0.01044691920352688</v>
+        <v>1.915839618896387</v>
       </c>
       <c r="I33">
-        <v>0.01061616204509746</v>
+        <v>1.946876725126332</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1486,13 +1486,13 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <v>0.002375522614975295</v>
+        <v>1.141733181299886</v>
       </c>
       <c r="H34">
-        <v>0.00394200521921491</v>
+        <v>1.894622316479947</v>
       </c>
       <c r="I34">
-        <v>0.00410386050157383</v>
+        <v>1.972413849708421</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1515,13 +1515,13 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <v>0.0009076189162304044</v>
+        <v>1.130894077242</v>
       </c>
       <c r="H35">
-        <v>0.00152338007571199</v>
+        <v>1.898133097717215</v>
       </c>
       <c r="I35">
-        <v>0.00159000459511328</v>
+        <v>1.981147315515742</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1544,13 +1544,13 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <v>0.0003497300783255483</v>
+        <v>1.145730075527708</v>
       </c>
       <c r="H36">
-        <v>0.0005859061448664661</v>
+        <v>1.919452552734483</v>
       </c>
       <c r="I36">
-        <v>0.0006090464099454843</v>
+        <v>1.995261009884215</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1573,13 +1573,13 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <v>0.0001346127829644831</v>
+        <v>1.14347865007609</v>
       </c>
       <c r="H37">
-        <v>0.0002302308271249672</v>
+        <v>1.955713488786722</v>
       </c>
       <c r="I37">
-        <v>0.0002348559041600026</v>
+        <v>1.995001561791762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>